<commit_message>
Moving back to UoU PC to check out files on larger screen.
</commit_message>
<xml_diff>
--- a/data/model/conical_r_70.0_linear.xlsx
+++ b/data/model/conical_r_70.0_linear.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\GitHub\NN_TiAlTa\data\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joe/GitHub/NN_TiAlTa/data/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72FA5AF-F8FC-43FB-85F5-A799C82E09E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EE7058-0D6E-594D-A026-D6E7F7635D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{22A46240-1FAA-4683-91B8-CDEDEB32A322}"/>
+    <workbookView xWindow="13820" yWindow="1560" windowWidth="28800" windowHeight="13620" xr2:uid="{22A46240-1FAA-4683-91B8-CDEDEB32A322}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -72,11 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -95,9 +105,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -135,7 +145,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -241,7 +251,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -383,7 +393,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -393,13 +403,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1830E8A8-A2DA-40CF-AFFA-FCF2BEB6AEEF}">
   <dimension ref="A1:DT158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DP1" workbookViewId="0">
-      <selection activeCell="DW10" sqref="DW10"/>
+    <sheetView tabSelected="1" topLeftCell="DI1" workbookViewId="0">
+      <selection activeCell="DP12" sqref="DP12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0.22600000000000001</v>
       </c>
@@ -430,7 +440,7 @@
       <c r="V1">
         <v>5</v>
       </c>
-      <c r="Z1" s="3">
+      <c r="Z1">
         <v>0.20599999999999999</v>
       </c>
       <c r="AA1">
@@ -551,7 +561,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>0.001*B107/A107^2</f>
         <v>487.33684135510225</v>
@@ -853,357 +863,309 @@
         <v>0.4717533538596877</v>
       </c>
     </row>
-    <row r="3" spans="1:124" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:124" x14ac:dyDescent="0.2">
+      <c r="A3">
         <f>MAX(A5:A158)</f>
         <v>0.15986</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <f>MAX(B5:B158)</f>
         <v>12454</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <f>MAX(C5:C158)</f>
         <v>882.5</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2">
+      <c r="F3">
         <f>MAX(F5:F158)</f>
         <v>0.17071</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <f>MAX(G5:G158)</f>
         <v>13147</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <f>MAX(H5:H158)</f>
         <v>993.41</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2">
+      <c r="K3">
         <f>MAX(K5:K158)</f>
         <v>0.18157999999999999</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3">
         <f>MAX(L5:L158)</f>
         <v>13830</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3">
         <f>MAX(M5:M158)</f>
         <v>1110.5</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2">
+      <c r="P3">
         <f>MAX(P5:P158)</f>
         <v>0.19244</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3">
         <f>MAX(Q5:Q158)</f>
         <v>14501</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3">
         <f>MAX(R5:R158)</f>
         <v>1233.9000000000001</v>
       </c>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2">
+      <c r="U3">
         <f>MAX(U5:U158)</f>
         <v>0.14901</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3">
         <f>MAX(V5:V158)</f>
         <v>11758</v>
       </c>
-      <c r="W3" s="2">
+      <c r="W3">
         <f>MAX(W5:W158)</f>
         <v>777.67</v>
       </c>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2">
+      <c r="Z3">
         <f>MAX(Z5:Z158)</f>
         <v>0.13814000000000001</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA3">
         <f>MAX(AA5:AA158)</f>
         <v>11051</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AB3">
         <f>MAX(AB5:AB158)</f>
         <v>679.03</v>
       </c>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2">
+      <c r="AE3">
         <f>MAX(AE5:AE158)</f>
         <v>0.12726999999999999</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AF3">
         <f>MAX(AF5:AF158)</f>
         <v>10345</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="AG3">
         <f>MAX(AG5:AG158)</f>
         <v>586.46</v>
       </c>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2">
+      <c r="AJ3">
         <f>MAX(AJ5:AJ158)</f>
         <v>0.11638999999999999</v>
       </c>
-      <c r="AK3" s="2">
+      <c r="AK3">
         <f>MAX(AK5:AK158)</f>
         <v>9624.2999999999993</v>
       </c>
-      <c r="AL3" s="2">
+      <c r="AL3">
         <f>MAX(AL5:AL158)</f>
         <v>500.18</v>
       </c>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2">
+      <c r="AO3">
         <f>MAX(AO5:AO158)</f>
         <v>0.1055</v>
       </c>
-      <c r="AP3" s="2">
+      <c r="AP3">
         <f>MAX(AP5:AP158)</f>
         <v>8890.2000000000007</v>
       </c>
-      <c r="AQ3" s="2">
+      <c r="AQ3">
         <f>MAX(AQ5:AQ158)</f>
         <v>420.37</v>
       </c>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2">
+      <c r="AT3">
         <f>MAX(AT5:AT158)</f>
         <v>9.4617000000000007E-2</v>
       </c>
-      <c r="AU3" s="2">
+      <c r="AU3">
         <f>MAX(AU5:AU158)</f>
         <v>8157.6</v>
       </c>
-      <c r="AV3" s="2">
+      <c r="AV3">
         <f>MAX(AV5:AV158)</f>
         <v>346.84</v>
       </c>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2"/>
-      <c r="AY3" s="2">
+      <c r="AY3">
         <f>MAX(AY5:AY158)</f>
         <v>8.3737000000000006E-2</v>
       </c>
-      <c r="AZ3" s="2">
+      <c r="AZ3">
         <f>MAX(AZ5:AZ158)</f>
         <v>7424</v>
       </c>
-      <c r="BA3" s="2">
+      <c r="BA3">
         <f>MAX(BA5:BA158)</f>
         <v>279.68</v>
       </c>
-      <c r="BB3" s="2"/>
-      <c r="BC3" s="2"/>
-      <c r="BD3" s="2">
+      <c r="BD3">
         <f>MAX(BD5:BD158)</f>
         <v>7.2858999999999993E-2</v>
       </c>
-      <c r="BE3" s="2">
+      <c r="BE3">
         <f>MAX(BE5:BE158)</f>
         <v>6675</v>
       </c>
-      <c r="BF3" s="2">
+      <c r="BF3">
         <f>MAX(BF5:BF158)</f>
         <v>219.02</v>
       </c>
-      <c r="BG3" s="2"/>
-      <c r="BH3" s="2"/>
-      <c r="BI3" s="2">
+      <c r="BI3">
         <f>MAX(BI5:BI158)</f>
         <v>6.1989000000000002E-2</v>
       </c>
-      <c r="BJ3" s="2">
+      <c r="BJ3">
         <f>MAX(BJ5:BJ158)</f>
         <v>5911.5</v>
       </c>
-      <c r="BK3" s="2">
+      <c r="BK3">
         <f>MAX(BK5:BK158)</f>
         <v>164.92</v>
       </c>
-      <c r="BL3" s="2"/>
-      <c r="BM3" s="2"/>
-      <c r="BN3" s="2">
+      <c r="BN3">
         <f>MAX(BN5:BN158)</f>
         <v>6.7416000000000004E-2</v>
       </c>
-      <c r="BO3" s="2">
+      <c r="BO3">
         <f>MAX(BO5:BO158)</f>
         <v>6300.8</v>
       </c>
-      <c r="BP3" s="2">
+      <c r="BP3">
         <f>MAX(BP5:BP158)</f>
         <v>191.08</v>
       </c>
-      <c r="BQ3" s="2"/>
-      <c r="BR3" s="2"/>
-      <c r="BS3" s="2">
+      <c r="BS3">
         <f>MAX(BS5:BS158)</f>
         <v>4.0288999999999998E-2</v>
       </c>
-      <c r="BT3" s="2">
+      <c r="BT3">
         <f>MAX(BT5:BT158)</f>
         <v>4322.8</v>
       </c>
-      <c r="BU3" s="2">
+      <c r="BU3">
         <f>MAX(BU5:BU158)</f>
         <v>77.143000000000001</v>
       </c>
-      <c r="BV3" s="2"/>
-      <c r="BW3" s="2"/>
-      <c r="BX3" s="2">
+      <c r="BX3">
         <f>MAX(BX5:BX158)</f>
         <v>5.1136000000000001E-2</v>
       </c>
-      <c r="BY3" s="2">
+      <c r="BY3">
         <f>MAX(BY5:BY158)</f>
         <v>5124.3999999999996</v>
       </c>
-      <c r="BZ3" s="2">
+      <c r="BZ3">
         <f>MAX(BZ5:BZ158)</f>
         <v>117.66</v>
       </c>
-      <c r="CA3" s="2"/>
-      <c r="CB3" s="2"/>
-      <c r="CC3" s="2">
+      <c r="CC3">
         <f>MAX(CC5:CC158)</f>
         <v>4.5704000000000002E-2</v>
       </c>
-      <c r="CD3" s="2">
+      <c r="CD3">
         <f>MAX(CD5:CD158)</f>
         <v>4731.2</v>
       </c>
-      <c r="CE3" s="2">
+      <c r="CE3">
         <f>MAX(CE5:CE158)</f>
         <v>96.525000000000006</v>
       </c>
-      <c r="CF3" s="2"/>
-      <c r="CG3" s="2"/>
-      <c r="CH3" s="2">
+      <c r="CH3">
         <f>MAX(CH5:CH158)</f>
         <v>5.6564000000000003E-2</v>
       </c>
-      <c r="CI3" s="2">
+      <c r="CI3">
         <f>MAX(CI5:CI158)</f>
         <v>5517.8</v>
       </c>
-      <c r="CJ3" s="2">
+      <c r="CJ3">
         <f>MAX(CJ5:CJ158)</f>
         <v>140.46</v>
       </c>
-      <c r="CK3" s="2"/>
-      <c r="CL3" s="2"/>
-      <c r="CM3" s="2">
+      <c r="CM3">
         <f>MAX(CM5:CM158)</f>
         <v>7.8298999999999994E-2</v>
       </c>
-      <c r="CN3" s="2">
+      <c r="CN3">
         <f>MAX(CN5:CN158)</f>
         <v>7049.4</v>
       </c>
-      <c r="CO3" s="2">
+      <c r="CO3">
         <f>MAX(CO5:CO158)</f>
         <v>248.55</v>
       </c>
-      <c r="CP3" s="2"/>
-      <c r="CQ3" s="2"/>
-      <c r="CR3" s="2">
+      <c r="CR3">
         <f>MAX(CR5:CR158)</f>
         <v>8.9177000000000006E-2</v>
       </c>
-      <c r="CS3" s="2">
+      <c r="CS3">
         <f>MAX(CS5:CS158)</f>
         <v>7792.3</v>
       </c>
-      <c r="CT3" s="2">
+      <c r="CT3">
         <f>MAX(CT5:CT158)</f>
         <v>312.45999999999998</v>
       </c>
-      <c r="CU3" s="2"/>
-      <c r="CV3" s="2"/>
-      <c r="CW3" s="1">
+      <c r="CW3" s="2">
         <f>MAX(CW5:CW158)</f>
         <v>0.10006</v>
       </c>
-      <c r="CX3" s="2">
+      <c r="CX3">
         <f>MAX(CX5:CX158)</f>
         <v>8523.6</v>
       </c>
-      <c r="CY3" s="2">
+      <c r="CY3">
         <f>MAX(CY5:CY158)</f>
         <v>382.81</v>
       </c>
-      <c r="CZ3" s="2"/>
-      <c r="DA3" s="2"/>
-      <c r="DB3" s="2">
+      <c r="DB3">
         <f>MAX(DB5:DB158)</f>
         <v>0.11094999999999999</v>
       </c>
-      <c r="DC3" s="2">
+      <c r="DC3">
         <f>MAX(DC5:DC158)</f>
         <v>9257.1</v>
       </c>
-      <c r="DD3" s="2">
+      <c r="DD3">
         <f>MAX(DD5:DD158)</f>
         <v>459.49</v>
       </c>
-      <c r="DE3" s="2"/>
-      <c r="DF3" s="2"/>
-      <c r="DG3" s="2">
+      <c r="DG3">
         <f>MAX(DG5:DG158)</f>
         <v>0.12182999999999999</v>
       </c>
-      <c r="DH3" s="2">
+      <c r="DH3">
         <f>MAX(DH5:DH158)</f>
         <v>9991.2999999999993</v>
       </c>
-      <c r="DI3" s="2">
+      <c r="DI3">
         <f>MAX(DI5:DI158)</f>
         <v>542.44000000000005</v>
       </c>
-      <c r="DJ3" s="2"/>
-      <c r="DK3" s="2"/>
-      <c r="DL3" s="2">
+      <c r="DL3">
         <f>MAX(DL5:DL158)</f>
         <v>0.13270999999999999</v>
       </c>
-      <c r="DM3" s="2">
+      <c r="DM3">
         <f>MAX(DM5:DM158)</f>
         <v>10697</v>
       </c>
-      <c r="DN3" s="2">
+      <c r="DN3">
         <f>MAX(DN5:DN158)</f>
         <v>631.99</v>
       </c>
-      <c r="DO3" s="2"/>
-      <c r="DP3" s="2"/>
-      <c r="DQ3" s="2">
+      <c r="DQ3">
         <f>MAX(DQ5:DQ158)</f>
         <v>0.14358000000000001</v>
       </c>
-      <c r="DR3" s="2">
+      <c r="DR3">
         <f>MAX(DR5:DR158)</f>
         <v>11405</v>
       </c>
-      <c r="DS3" s="2">
+      <c r="DS3">
         <f>MAX(DS5:DS158)</f>
         <v>727.59</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1505,7 +1467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -1807,7 +1769,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -2109,7 +2071,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -2411,7 +2373,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -2713,7 +2675,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -3015,7 +2977,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -3317,7 +3279,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -3619,7 +3581,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -3921,7 +3883,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -4223,7 +4185,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="14" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -4525,7 +4487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -4827,7 +4789,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -5129,7 +5091,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -5431,7 +5393,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="18" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -5733,7 +5695,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="19" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -6035,7 +5997,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -6337,7 +6299,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="21" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -6639,7 +6601,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="22" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -6941,7 +6903,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="23" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -7243,7 +7205,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="24" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -7545,7 +7507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -7847,7 +7809,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="26" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -8149,7 +8111,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -8451,7 +8413,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -8753,7 +8715,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="29" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -9055,7 +9017,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -9357,7 +9319,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="31" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>0</v>
       </c>
@@ -9659,7 +9621,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="32" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -9961,7 +9923,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="33" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -10263,7 +10225,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="34" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -10565,7 +10527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>0</v>
       </c>
@@ -10867,7 +10829,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="36" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>0</v>
       </c>
@@ -11169,7 +11131,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="37" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>0</v>
       </c>
@@ -11471,7 +11433,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="38" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2.8336000000000002E-4</v>
       </c>
@@ -11773,7 +11735,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="39" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2.4873E-3</v>
       </c>
@@ -12075,7 +12037,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="40" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>4.6901E-3</v>
       </c>
@@ -12377,7 +12339,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="41" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>6.8916999999999997E-3</v>
       </c>
@@ -12679,7 +12641,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="42" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>9.0921999999999999E-3</v>
       </c>
@@ -12981,7 +12943,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="43" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>1.1292E-2</v>
       </c>
@@ -13283,7 +13245,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="44" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>1.349E-2</v>
       </c>
@@ -13585,7 +13547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>1.5778E-2</v>
       </c>
@@ -13887,7 +13849,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>1.8072000000000001E-2</v>
       </c>
@@ -14189,7 +14151,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="47" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2.0379999999999999E-2</v>
       </c>
@@ -14491,7 +14453,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="48" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2.2724999999999999E-2</v>
       </c>
@@ -14793,7 +14755,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2.5072000000000001E-2</v>
       </c>
@@ -15095,7 +15057,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="50" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2.7418000000000001E-2</v>
       </c>
@@ -15397,7 +15359,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2.9787999999999999E-2</v>
       </c>
@@ -15699,7 +15661,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="52" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>3.2212999999999999E-2</v>
       </c>
@@ -16001,7 +15963,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="53" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>3.4637000000000001E-2</v>
       </c>
@@ -16303,7 +16265,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="54" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>3.7060000000000003E-2</v>
       </c>
@@ -16605,7 +16567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>3.9490999999999998E-2</v>
       </c>
@@ -16907,7 +16869,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="56" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>4.1925999999999998E-2</v>
       </c>
@@ -17209,7 +17171,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="57" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>4.4375999999999999E-2</v>
       </c>
@@ -17511,7 +17473,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="58" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>4.6833E-2</v>
       </c>
@@ -17813,7 +17775,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="59" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>4.9287999999999998E-2</v>
       </c>
@@ -18115,7 +18077,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>5.1743999999999998E-2</v>
       </c>
@@ -18417,7 +18379,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="61" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>5.4197000000000002E-2</v>
       </c>
@@ -18719,7 +18681,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="62" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>5.6649999999999999E-2</v>
       </c>
@@ -19021,7 +18983,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="63" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>5.9103000000000003E-2</v>
       </c>
@@ -19323,7 +19285,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="64" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>6.1553999999999998E-2</v>
       </c>
@@ -19625,7 +19587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>6.4005000000000006E-2</v>
       </c>
@@ -19927,7 +19889,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="66" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>6.6458000000000003E-2</v>
       </c>
@@ -20229,7 +20191,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="67" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>6.8916000000000005E-2</v>
       </c>
@@ -20531,7 +20493,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="68" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>7.1376999999999996E-2</v>
       </c>
@@ -20833,7 +20795,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="69" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>7.3837E-2</v>
       </c>
@@ -21135,7 +21097,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="70" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>7.6296000000000003E-2</v>
       </c>
@@ -21437,7 +21399,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="71" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>7.8755000000000006E-2</v>
       </c>
@@ -21739,7 +21701,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="72" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>8.1212999999999994E-2</v>
       </c>
@@ -22041,7 +22003,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="73" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>8.3669999999999994E-2</v>
       </c>
@@ -22343,7 +22305,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="74" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>8.6127999999999996E-2</v>
       </c>
@@ -22645,7 +22607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>8.8586999999999999E-2</v>
       </c>
@@ -22947,7 +22909,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="76" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>9.1047000000000003E-2</v>
       </c>
@@ -23249,7 +23211,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="77" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>9.3506000000000006E-2</v>
       </c>
@@ -23551,7 +23513,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="78" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>9.5963999999999994E-2</v>
       </c>
@@ -23853,7 +23815,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="79" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>9.8422999999999997E-2</v>
       </c>
@@ -24155,7 +24117,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="80" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>0.10088999999999999</v>
       </c>
@@ -24457,7 +24419,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="81" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>0.10335</v>
       </c>
@@ -24759,7 +24721,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="82" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>0.10581</v>
       </c>
@@ -25061,7 +25023,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="83" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>0.10827000000000001</v>
       </c>
@@ -25363,7 +25325,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="84" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>0.11073</v>
       </c>
@@ -25665,7 +25627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>0.11319</v>
       </c>
@@ -25967,7 +25929,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="86" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>0.11565</v>
       </c>
@@ -26269,7 +26231,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="87" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>0.11811000000000001</v>
       </c>
@@ -26571,7 +26533,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="88" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>0.12056</v>
       </c>
@@ -26873,7 +26835,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="89" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>0.12302</v>
       </c>
@@ -27175,7 +27137,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="90" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>0.12548000000000001</v>
       </c>
@@ -27477,7 +27439,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="91" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>0.12794</v>
       </c>
@@ -27779,7 +27741,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="92" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>0.13039999999999999</v>
       </c>
@@ -28081,7 +28043,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="93" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>0.13286000000000001</v>
       </c>
@@ -28383,7 +28345,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="94" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>0.13531000000000001</v>
       </c>
@@ -28685,7 +28647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>0.13777</v>
       </c>
@@ -28987,7 +28949,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="96" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>0.14022999999999999</v>
       </c>
@@ -29289,7 +29251,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="97" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>0.14268</v>
       </c>
@@ -29591,7 +29553,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="98" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>0.14513999999999999</v>
       </c>
@@ -29893,7 +29855,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="99" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>0.14759</v>
       </c>
@@ -30195,7 +30157,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="100" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>0.15004999999999999</v>
       </c>
@@ -30497,7 +30459,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="101" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>0.1525</v>
       </c>
@@ -30799,7 +30761,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="102" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>0.15495999999999999</v>
       </c>
@@ -31101,7 +31063,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="103" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>0.15740999999999999</v>
       </c>
@@ -31403,7 +31365,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="104" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>0.15986</v>
       </c>
@@ -31705,7 +31667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>0.15986</v>
       </c>
@@ -32007,7 +31969,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>0.15986</v>
       </c>
@@ -32309,7 +32271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>0.15986</v>
       </c>
@@ -32611,7 +32573,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="108" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>0.15986</v>
       </c>
@@ -32913,7 +32875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>0.15554000000000001</v>
       </c>
@@ -33215,7 +33177,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="110" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>0.15121000000000001</v>
       </c>
@@ -33517,7 +33479,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="111" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>0.14688000000000001</v>
       </c>
@@ -33819,7 +33781,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="112" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>0.14255000000000001</v>
       </c>
@@ -34121,7 +34083,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="113" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>0.13822000000000001</v>
       </c>
@@ -34423,7 +34385,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>0.13389000000000001</v>
       </c>
@@ -34725,7 +34687,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="115" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>0.12955</v>
       </c>
@@ -35027,7 +34989,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>0.12522</v>
       </c>
@@ -35329,7 +35291,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>0.12089999999999999</v>
       </c>
@@ -35631,7 +35593,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="118" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>0.11656999999999999</v>
       </c>
@@ -35933,7 +35895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>0.11224000000000001</v>
       </c>
@@ -36235,7 +36197,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="120" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>0.10791000000000001</v>
       </c>
@@ -36537,7 +36499,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>0.10357</v>
       </c>
@@ -36839,7 +36801,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>9.9237000000000006E-2</v>
       </c>
@@ -37141,7 +37103,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="123" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>9.4895999999999994E-2</v>
       </c>
@@ -37443,7 +37405,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>9.0552999999999995E-2</v>
       </c>
@@ -37745,7 +37707,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="125" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>8.6206000000000005E-2</v>
       </c>
@@ -38047,7 +38009,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>8.1855999999999998E-2</v>
       </c>
@@ -38349,7 +38311,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="127" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>7.7503000000000002E-2</v>
       </c>
@@ -38651,7 +38613,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="128" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>7.3146000000000003E-2</v>
       </c>
@@ -38953,7 +38915,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>6.8786E-2</v>
       </c>
@@ -39255,7 +39217,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="130" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>6.8289000000000002E-2</v>
       </c>
@@ -39557,7 +39519,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -39859,7 +39821,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -40161,7 +40123,7 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="133" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -40463,7 +40425,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -40765,7 +40727,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="135" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -41067,7 +41029,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -41369,7 +41331,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="137" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -41671,7 +41633,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="138" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -41973,7 +41935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="139" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -42275,7 +42237,7 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="140" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -42577,7 +42539,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="141" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -42879,7 +42841,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="142" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -43181,7 +43143,7 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="143" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -43483,7 +43445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="144" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -43785,7 +43747,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="145" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -44087,7 +44049,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="146" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -44389,7 +44351,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="147" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -44691,7 +44653,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="148" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -44993,7 +44955,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -45295,7 +45257,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="150" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -45597,7 +45559,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="151" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -45899,7 +45861,7 @@
         <v>23.6</v>
       </c>
     </row>
-    <row r="152" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -46201,7 +46163,7 @@
         <v>23.8</v>
       </c>
     </row>
-    <row r="153" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -46503,7 +46465,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="154" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -46805,7 +46767,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="155" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -47107,7 +47069,7 @@
         <v>24.4</v>
       </c>
     </row>
-    <row r="156" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -47409,7 +47371,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="157" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>6.8290000000000003E-2</v>
       </c>
@@ -47711,7 +47673,7 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="158" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>6.8290000000000003E-2</v>
       </c>

</xml_diff>